<commit_message>
Add source code, tests and pytest config for CI
</commit_message>
<xml_diff>
--- a/ドキュメント構成.xlsx
+++ b/ドキュメント構成.xlsx
@@ -2,18 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4cdcf9e0e0a4c38c/デスクトップ/Python練習用/yakkiho-checker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{9A00C416-FF5A-47FC-BA86-563069B30F3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AE2CE3C8-ACE1-4CB6-8EC8-58D824AACB1A}"/>
+  <xr:revisionPtr revIDLastSave="162" documentId="8_{9A00C416-FF5A-47FC-BA86-563069B30F3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{92F7461A-BFFA-4DA5-B913-DFA8C5C66927}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C016FA43-B9F7-47F2-9464-2D2B9D6BB813}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{C016FA43-B9F7-47F2-9464-2D2B9D6BB813}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="55">
   <si>
     <t>1. データ定義シート（m_Subcategories／m_Groups／Groups／Words）</t>
   </si>
@@ -147,12 +148,289 @@
     <t>Markdown テンプレート</t>
     <phoneticPr fontId="3"/>
   </si>
+  <si>
+    <t>1.プロジェクト概要と環境</t>
+  </si>
+  <si>
+    <t>主要なモジュール・ファイル一覧</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>NGワード処理ロジックスクリプト</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>UI管理スクリプト</t>
+    <rPh sb="2" eb="4">
+      <t>カンリ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>jsonの元データ1</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>ファイル名</t>
+    <rPh sb="4" eb="5">
+      <t>メイ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>内容</t>
+    <rPh sb="0" eb="2">
+      <t>ナイヨウ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>NGワードチェック用json
+「Ngwordマスタ.xlsm」「Markdown_texts」より作成</t>
+    <rPh sb="9" eb="10">
+      <t>ヨウ</t>
+    </rPh>
+    <rPh sb="49" eb="51">
+      <t>サクセイ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>jsonの元データ2
+サブカテゴリ毎に分かれたMarkdownファイル</t>
+    <rPh sb="17" eb="18">
+      <t>ゴト</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>ワ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>data_processing.py</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>ui.py</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>NGword.json</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>NGwordマスタ.xlsm</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>markdown_texts/（サブカテゴリ名）.md</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>分類</t>
+    <rPh sb="0" eb="2">
+      <t>ブンルイ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>config.py</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Ngword用プレースホルダー</t>
+    <rPh sb="6" eb="7">
+      <t>ヨウ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>アプリ用</t>
+    <rPh sb="3" eb="4">
+      <t>ヨウ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>json用</t>
+    <rPh sb="4" eb="5">
+      <t>ヨウ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>json_export_script.py</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>json生成スクリプト</t>
+    <rPh sb="4" eb="6">
+      <t>セイセイ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>デバッグ用</t>
+    <rPh sb="4" eb="5">
+      <t>ヨウ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>debug.log</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>バージョン：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Python 3.13.3</t>
+    </r>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>フレームワーク：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Streamlit</t>
+    </r>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ディレクトリ構成：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>C:\Users\harum\OneDrive\デスクトップ\Python練習用\yakkiho-checker</t>
+    </r>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Ngwordマスタ用</t>
+    <rPh sb="9" eb="10">
+      <t>ヨウ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Master_Update.py</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>NGwordマスター自動更新スクリプト
+Excel内で自動更新できるので、不要かと思われるが、以下の点で利用価値ありそうなので、一旦残す。
+　・Excel を開けない環境（サーバー上で完全自動化したい）
+　・Power Query では表現しづらい複雑なロジック（例えば日付条件や文字列操作を Python で一括処理したい）
+　・ユーザー操作を極力省きたい（Windowsタスクスケジューラや CI/CD に組み込みたい）</t>
+    <rPh sb="20" eb="26">
+      <t>エクセルナイ</t>
+    </rPh>
+    <rPh sb="27" eb="29">
+      <t>ジドウ</t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t>コウシン</t>
+    </rPh>
+    <rPh sb="37" eb="39">
+      <t>フヨウ</t>
+    </rPh>
+    <rPh sb="41" eb="42">
+      <t>オモ</t>
+    </rPh>
+    <rPh sb="47" eb="49">
+      <t>イカ</t>
+    </rPh>
+    <rPh sb="50" eb="51">
+      <t>テン</t>
+    </rPh>
+    <rPh sb="52" eb="56">
+      <t>リヨウカチ</t>
+    </rPh>
+    <rPh sb="64" eb="66">
+      <t>イッタン</t>
+    </rPh>
+    <rPh sb="66" eb="67">
+      <t>ノコ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>テスト用</t>
+    <rPh sb="3" eb="4">
+      <t>ヨウ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>test_data_processing.py</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>"data_processing.py"用のテストスクリプト</t>
+    <rPh sb="20" eb="21">
+      <t>ヨウ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -193,16 +471,39 @@
       <name val="Segoe UI Emoji"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -210,13 +511,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -228,6 +544,36 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -542,10 +888,183 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E439906-1CF8-4371-851F-FE1C8EC32A51}">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="16.5" customWidth="1"/>
+    <col min="2" max="2" width="35.796875" customWidth="1"/>
+    <col min="3" max="3" width="93.19921875" customWidth="1"/>
+    <col min="4" max="4" width="37.3984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="22.2" x14ac:dyDescent="0.45">
+      <c r="A1" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="22.2" x14ac:dyDescent="0.45">
+      <c r="A2" s="8"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A3" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A5" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A6" s="9"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A7" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A8" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A9" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A10" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="36" x14ac:dyDescent="0.45">
+      <c r="A11" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A12" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A13" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="36" x14ac:dyDescent="0.45">
+      <c r="A14" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A15" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="90" x14ac:dyDescent="0.45">
+      <c r="A16" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A17" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="5"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A18" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4112C19-DE84-47D5-BDA7-08C0083481A0}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>

</xml_diff>